<commit_message>
WIP Creating final graphs.
</commit_message>
<xml_diff>
--- a/data/processed/df_after_preprocessing_MEXIDO.xlsx
+++ b/data/processed/df_after_preprocessing_MEXIDO.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJETOS NO GIT\ethereum_laundering\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDCB1B5-EC48-4B7C-B04A-1B76CFB57D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA86F44-CE86-4F1E-A887-23C2ABE1A064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODAS AS COLUNAS" sheetId="1" r:id="rId1"/>
     <sheet name="SOMENTE ALTERADAS" sheetId="2" r:id="rId2"/>
+    <sheet name="Testing dataset" sheetId="3" r:id="rId3"/>
+    <sheet name="train_cat" sheetId="4" r:id="rId4"/>
+    <sheet name="test_cat" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SOMENTE ALTERADAS'!$A$2:$I$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SOMENTE ALTERADAS'!$A$2:$G$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t>Avg_min_between_sent_tnx</t>
   </si>
@@ -167,7 +170,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -206,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -255,30 +258,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -298,20 +277,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,37 +373,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I28" sqref="A28:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,75 +690,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="13">
-        <v>3975</v>
-      </c>
-      <c r="C3" s="13">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
+        <v>3975</v>
+      </c>
+      <c r="C3" s="9">
         <v>3451.928067924528</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="9">
         <v>16526.435570519741</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="9">
         <v>3.26</v>
       </c>
-      <c r="F3" s="13">
-        <v>3975</v>
-      </c>
-      <c r="G3" s="13">
+      <c r="F3" s="9">
+        <v>3975</v>
+      </c>
+      <c r="G3" s="9">
         <v>3451.928067924528</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="9">
         <v>16526.435570519741</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="9">
         <v>3.26</v>
       </c>
       <c r="J3" t="b">
@@ -758,31 +778,31 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C4" s="10">
         <v>5240.4822515723272</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="10">
         <v>18552.810463429782</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="10">
         <v>93.49</v>
       </c>
-      <c r="F4" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G4" s="14">
+      <c r="F4" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G4" s="10">
         <v>5240.4822515723272</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="10">
         <v>18552.810463429782</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="10">
         <v>93.49</v>
       </c>
       <c r="J4" t="b">
@@ -803,31 +823,31 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15">
-        <v>3975</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="B5" s="11">
+        <v>3975</v>
+      </c>
+      <c r="C5" s="11">
         <v>132036.15236981129</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <v>242657.58168036511</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <v>10561.05</v>
       </c>
-      <c r="F5" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G5" s="15">
+      <c r="F5" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G5" s="11">
         <v>132036.15236981129</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="11">
         <v>242657.58168036511</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <v>10561.05</v>
       </c>
       <c r="J5" t="b">
@@ -848,31 +868,31 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C6" s="14">
+      <c r="B6" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C6" s="10">
         <v>90.188176100628937</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="10">
         <v>737.60948216125951</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="10">
         <v>2</v>
       </c>
-      <c r="F6" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G6" s="14">
+      <c r="F6" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G6" s="10">
         <v>90.188176100628937</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="10">
         <v>737.60948216125951</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="10">
         <v>2</v>
       </c>
       <c r="J6" t="b">
@@ -893,31 +913,31 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15">
-        <v>3975</v>
-      </c>
-      <c r="C7" s="15">
+      <c r="B7" s="11">
+        <v>3975</v>
+      </c>
+      <c r="C7" s="11">
         <v>181.94716981132069</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="11">
         <v>1123.4421081362329</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="11">
         <v>3</v>
       </c>
-      <c r="F7" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G7" s="15">
+      <c r="F7" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G7" s="11">
         <v>181.94716981132069</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="11">
         <v>1123.4421081362329</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="11">
         <v>3</v>
       </c>
       <c r="J7" t="b">
@@ -938,31 +958,31 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C8" s="14">
+      <c r="B8" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C8" s="10">
         <v>5.8070440251572331</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="10">
         <v>201.28645456121899</v>
       </c>
-      <c r="E8" s="14">
-        <v>0</v>
-      </c>
-      <c r="F8" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G8" s="14">
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G8" s="10">
         <v>5.8070440251572331</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="10">
         <v>201.28645456121899</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="10">
         <v>0</v>
       </c>
       <c r="J8" t="b">
@@ -983,31 +1003,31 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15">
-        <v>3975</v>
-      </c>
-      <c r="C9" s="15">
+      <c r="B9" s="11">
+        <v>3975</v>
+      </c>
+      <c r="C9" s="11">
         <v>40.510943396226423</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="11">
         <v>325.24366742380391</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="11">
         <v>2</v>
       </c>
-      <c r="F9" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G9" s="15">
+      <c r="F9" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G9" s="11">
         <v>40.510943396226423</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="11">
         <v>325.24366742380391</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="11">
         <v>2</v>
       </c>
       <c r="J9" t="b">
@@ -1028,31 +1048,31 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C10" s="14">
+      <c r="B10" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C10" s="10">
         <v>25.429433962264149</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="10">
         <v>255.69882138215269</v>
       </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G10" s="14">
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G10" s="10">
         <v>25.429433962264149</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="10">
         <v>255.69882138215269</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="10">
         <v>1</v>
       </c>
       <c r="J10" t="b">
@@ -1073,31 +1093,31 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="15">
-        <v>3975</v>
-      </c>
-      <c r="C11" s="15">
+      <c r="B11" s="11">
+        <v>3975</v>
+      </c>
+      <c r="C11" s="11">
         <v>50.227133266666669</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="11">
         <v>463.53259623186409</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="11">
         <v>4.6531000000000003E-2</v>
       </c>
-      <c r="F11" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G11" s="15">
+      <c r="F11" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G11" s="11">
         <v>50.227133266666669</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="11">
         <v>463.53259623186409</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="11">
         <v>4.6531000000000003E-2</v>
       </c>
       <c r="J11" t="b">
@@ -1118,31 +1138,31 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C12" s="14">
+      <c r="B12" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C12" s="10">
         <v>842.61445406641519</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="10">
         <v>18970.780595194821</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="10">
         <v>4</v>
       </c>
-      <c r="F12" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G12" s="14">
+      <c r="F12" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G12" s="10">
         <v>842.61445406641519</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="10">
         <v>18970.780595194821</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="10">
         <v>4</v>
       </c>
       <c r="J12" t="b">
@@ -1163,31 +1183,31 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="15">
-        <v>3975</v>
-      </c>
-      <c r="C13" s="15">
+      <c r="B13" s="11">
+        <v>3975</v>
+      </c>
+      <c r="C13" s="11">
         <v>148.65226063119499</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <v>4529.8602729491968</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="11">
         <v>1.05</v>
       </c>
-      <c r="F13" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G13" s="15">
+      <c r="F13" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G13" s="11">
         <v>148.65226063119499</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="11">
         <v>4529.8602729491968</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="11">
         <v>1.05</v>
       </c>
       <c r="J13" t="b">
@@ -1208,31 +1228,31 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C14" s="14">
+      <c r="B14" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C14" s="10">
         <v>5.0461193451572326</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="10">
         <v>82.578319813416911</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="10">
         <v>5.8058999999999999E-2</v>
       </c>
-      <c r="F14" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G14" s="14">
+      <c r="F14" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G14" s="10">
         <v>5.0461193451572326</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="10">
         <v>82.578319813416911</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="10">
         <v>5.8058999999999999E-2</v>
       </c>
       <c r="J14" t="b">
@@ -1253,31 +1273,31 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="15">
-        <v>3975</v>
-      </c>
-      <c r="C15" s="15">
+      <c r="B15" s="11">
+        <v>3975</v>
+      </c>
+      <c r="C15" s="11">
         <v>466.68768049006292</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="11">
         <v>10090.138360408489</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="11">
         <v>2.8830529999999999</v>
       </c>
-      <c r="F15" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G15" s="15">
+      <c r="F15" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G15" s="11">
         <v>466.68768049006292</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="11">
         <v>10090.138360408489</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="11">
         <v>2.8830529999999999</v>
       </c>
       <c r="J15" t="b">
@@ -1298,31 +1318,31 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C16" s="14">
+      <c r="B16" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C16" s="10">
         <v>38.035581045534592</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="10">
         <v>242.43914898483749</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="10">
         <v>1.2445170000000001</v>
       </c>
-      <c r="F16" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G16" s="14">
+      <c r="F16" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G16" s="10">
         <v>38.035581045534592</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="10">
         <v>242.43914898483749</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="10">
         <v>1.2445170000000001</v>
       </c>
       <c r="J16" t="b">
@@ -1343,31 +1363,31 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="15">
-        <v>3975</v>
-      </c>
-      <c r="C17" s="15">
+      <c r="B17" s="11">
+        <v>3975</v>
+      </c>
+      <c r="C17" s="11">
         <v>277.9423899371069</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="11">
         <v>1474.252547456083</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="11">
         <v>6</v>
       </c>
-      <c r="F17" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G17" s="15">
+      <c r="F17" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G17" s="11">
         <v>277.9423899371069</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="11">
         <v>1474.252547456083</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="11">
         <v>6</v>
       </c>
       <c r="J17" t="b">
@@ -1388,31 +1408,31 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C18" s="14">
+      <c r="B18" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C18" s="10">
         <v>9339.2233598925668</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="10">
         <v>278326.00132311549</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="10">
         <v>4.7171310000000002</v>
       </c>
-      <c r="F18" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G18" s="14">
+      <c r="F18" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G18" s="10">
         <v>9339.2233598925668</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="10">
         <v>278326.00132311549</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="10">
         <v>4.7171310000000002</v>
       </c>
       <c r="J18" t="b">
@@ -1433,31 +1453,31 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="15">
-        <v>3975</v>
-      </c>
-      <c r="C19" s="15">
+      <c r="B19" s="11">
+        <v>3975</v>
+      </c>
+      <c r="C19" s="11">
         <v>12463.34345432472</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="11">
         <v>296228.88973679318</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="11">
         <v>16.599058549999999</v>
       </c>
-      <c r="F19" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G19" s="15">
+      <c r="F19" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G19" s="11">
         <v>12463.34345432472</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="11">
         <v>296228.88973679318</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="11">
         <v>16.599058549999999</v>
       </c>
       <c r="J19" t="b">
@@ -1478,31 +1498,31 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="14">
-        <v>3975</v>
-      </c>
-      <c r="C20" s="14">
+      <c r="B20" s="10">
+        <v>3975</v>
+      </c>
+      <c r="C20" s="10">
         <v>3124.120094329156</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="10">
         <v>379907.65158953652</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="10">
         <v>1.5442559999999999E-3</v>
       </c>
-      <c r="F20" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G20" s="14">
+      <c r="F20" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G20" s="10">
         <v>3124.120094329156</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="10">
         <v>379907.65158953652</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="10">
         <v>1.5442559999999999E-3</v>
       </c>
       <c r="J20" t="b">
@@ -1523,31 +1543,31 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="11">
         <v>3264</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="11">
         <v>21.212316176470591</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="11">
         <v>261.88482393355378</v>
       </c>
-      <c r="E21" s="15">
-        <v>1</v>
-      </c>
-      <c r="F21" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G21" s="15">
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G21" s="11">
         <v>17.59698113207547</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="11">
         <v>237.43035975462209</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="11">
         <v>1</v>
       </c>
       <c r="J21" t="b">
@@ -1568,31 +1588,31 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="10">
         <v>3264</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="10">
         <v>330070050.22725868</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="10">
         <v>17509100558.713589</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="10">
         <v>1.337</v>
       </c>
-      <c r="F22" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G22" s="14">
+      <c r="F22" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G22" s="10">
         <v>271031105.63330311</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="10">
         <v>15866175331.40514</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="10">
         <v>1.337</v>
       </c>
       <c r="J22" t="b">
@@ -1613,31 +1633,31 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="11">
         <v>3264</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="11">
         <v>35107856.18864923</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="11">
         <v>1960481387.621767</v>
       </c>
-      <c r="E23" s="15">
-        <v>0</v>
-      </c>
-      <c r="F23" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G23" s="15">
+      <c r="E23" s="11">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G23" s="11">
         <v>28828186.817547441</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="11">
         <v>1776518720.275238</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I23" s="11">
         <v>0</v>
       </c>
       <c r="J23" t="b">
@@ -1658,31 +1678,31 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="10">
         <v>3264</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="10">
         <v>1.2928125619494799</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="10">
         <v>68.652184320815039</v>
       </c>
-      <c r="E24" s="14">
-        <v>0</v>
-      </c>
-      <c r="F24" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G24" s="14">
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G24" s="10">
         <v>1.06156986218946</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="10">
         <v>62.210364045706562</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="10">
         <v>0</v>
       </c>
       <c r="J24" t="b">
@@ -1703,31 +1723,31 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="11">
         <v>3264</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="11">
         <v>2.430759803921569</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="11">
         <v>41.249932815872953</v>
       </c>
-      <c r="E25" s="15">
-        <v>0</v>
-      </c>
-      <c r="F25" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G25" s="15">
+      <c r="E25" s="11">
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G25" s="11">
         <v>1.9959748427672961</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="11">
         <v>37.389763944295467</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="11">
         <v>0</v>
       </c>
       <c r="J25" t="b">
@@ -1748,31 +1768,31 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="10">
         <v>3264</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="10">
         <v>5.8927696078431371</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="10">
         <v>44.419987568039907</v>
       </c>
-      <c r="E26" s="14">
-        <v>1</v>
-      </c>
-      <c r="F26" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G26" s="14">
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G26" s="10">
         <v>5.0176100628930822</v>
       </c>
-      <c r="H26" s="14">
+      <c r="H26" s="10">
         <v>40.294327206900583</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="10">
         <v>1</v>
       </c>
       <c r="J26" t="b">
@@ -1793,31 +1813,31 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="11">
         <v>3264</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="11">
         <v>4.520833333333333</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="11">
         <v>16.485495285444578</v>
       </c>
-      <c r="E27" s="15">
-        <v>1</v>
-      </c>
-      <c r="F27" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G27" s="15">
+      <c r="E27" s="11">
+        <v>1</v>
+      </c>
+      <c r="F27" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G27" s="11">
         <v>3.8910691823899368</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="11">
         <v>14.998975245619789</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="11">
         <v>1</v>
       </c>
       <c r="J27" t="b">
@@ -1838,31 +1858,31 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="10">
         <v>3264</v>
       </c>
-      <c r="C28" s="14">
-        <v>0</v>
-      </c>
-      <c r="D28" s="14">
-        <v>0</v>
-      </c>
-      <c r="E28" s="14">
-        <v>0</v>
-      </c>
-      <c r="F28" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G28" s="14">
-        <v>0</v>
-      </c>
-      <c r="H28" s="14">
-        <v>0</v>
-      </c>
-      <c r="I28" s="14">
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10">
         <v>0</v>
       </c>
       <c r="J28" t="b">
@@ -1883,31 +1903,31 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="11">
         <v>3264</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="11">
         <v>801.29755753707116</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="11">
         <v>21566.104021791991</v>
       </c>
-      <c r="E29" s="15">
-        <v>0</v>
-      </c>
-      <c r="F29" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G29" s="15">
+      <c r="E29" s="11">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G29" s="11">
         <v>657.97112649081771</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="11">
         <v>19544.291501904721</v>
       </c>
-      <c r="I29" s="15">
+      <c r="I29" s="11">
         <v>0</v>
       </c>
       <c r="J29" t="b">
@@ -1928,31 +1948,31 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="10">
         <v>3264</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="10">
         <v>324271708.62483138</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="10">
         <v>17508302812.896229</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="10">
         <v>1.337</v>
       </c>
-      <c r="F30" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G30" s="14">
+      <c r="F30" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G30" s="10">
         <v>266269901.35900801</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="10">
         <v>15865434919.82373</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="10">
         <v>1.337</v>
       </c>
       <c r="J30" t="b">
@@ -1973,31 +1993,31 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="11">
         <v>3264</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="11">
         <v>9158917.4188146573</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="11">
         <v>353764014.44052249</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="11">
         <v>0.86643500000000007</v>
       </c>
-      <c r="F31" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G31" s="15">
+      <c r="F31" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G31" s="11">
         <v>7520681.0241625998</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="11">
         <v>320578431.63703811</v>
       </c>
-      <c r="I31" s="15">
+      <c r="I31" s="11">
         <v>0.86643500000000007</v>
       </c>
       <c r="J31" t="b">
@@ -2018,31 +2038,31 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="10">
         <v>3264</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="10">
         <v>33599.78333427359</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="10">
         <v>1754378.05963397</v>
       </c>
-      <c r="E32" s="14">
-        <v>0</v>
-      </c>
-      <c r="F32" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G32" s="14">
+      <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G32" s="10">
         <v>27589.85982467145</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="10">
         <v>1589761.7496576849</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="10">
         <v>0</v>
       </c>
       <c r="J32" t="b">
@@ -2063,31 +2083,31 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="11">
         <v>3264</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="11">
         <v>34928920.87043152</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="11">
         <v>1960473669.1452661</v>
       </c>
-      <c r="E33" s="15">
-        <v>0</v>
-      </c>
-      <c r="F33" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G33" s="15">
+      <c r="E33" s="11">
+        <v>0</v>
+      </c>
+      <c r="F33" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G33" s="11">
         <v>28681257.288324151</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="11">
         <v>1776511208.2888081</v>
       </c>
-      <c r="I33" s="15">
+      <c r="I33" s="11">
         <v>0</v>
       </c>
       <c r="J33" t="b">
@@ -2108,31 +2128,31 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="10">
         <v>3264</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="10">
         <v>17378481.28444308</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="10">
         <v>982815117.76275134</v>
       </c>
-      <c r="E34" s="14">
-        <v>0</v>
-      </c>
-      <c r="F34" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G34" s="14">
+      <c r="E34" s="10">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10">
+        <v>3975</v>
+      </c>
+      <c r="G34" s="10">
         <v>14270028.405640811</v>
       </c>
-      <c r="H34" s="14">
+      <c r="H34" s="10">
         <v>890591572.66978121</v>
       </c>
-      <c r="I34" s="14">
+      <c r="I34" s="10">
         <v>0</v>
       </c>
       <c r="J34" t="b">
@@ -2153,31 +2173,31 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="11">
         <v>3264</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="11">
         <v>1.246936274509804</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="11">
         <v>6.3174516969443921</v>
       </c>
-      <c r="E35" s="15">
-        <v>0</v>
-      </c>
-      <c r="F35" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G35" s="15">
+      <c r="E35" s="11">
+        <v>0</v>
+      </c>
+      <c r="F35" s="11">
+        <v>3975</v>
+      </c>
+      <c r="G35" s="11">
         <v>1.0238993710691819</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="11">
         <v>5.7444034066363452</v>
       </c>
-      <c r="I35" s="15">
+      <c r="I35" s="11">
         <v>0</v>
       </c>
       <c r="J35" t="b">
@@ -2198,31 +2218,31 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="16">
+      <c r="B36" s="12">
         <v>3264</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="12">
         <v>4.465686274509804</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="12">
         <v>16.073423288550451</v>
       </c>
-      <c r="E36" s="16">
-        <v>1</v>
-      </c>
-      <c r="F36" s="16">
-        <v>3975</v>
-      </c>
-      <c r="G36" s="16">
+      <c r="E36" s="12">
+        <v>1</v>
+      </c>
+      <c r="F36" s="12">
+        <v>3975</v>
+      </c>
+      <c r="G36" s="12">
         <v>3.8457861635220132</v>
       </c>
-      <c r="H36" s="16">
+      <c r="H36" s="12">
         <v>14.625198925588821</v>
       </c>
-      <c r="I36" s="16">
+      <c r="I36" s="12">
         <v>1</v>
       </c>
       <c r="J36" t="b">
@@ -2253,506 +2273,1079 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61876367-A014-4DCE-9013-6625C8A49968}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="F2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="19" t="s">
+      <c r="G2" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="13">
         <v>3264</v>
       </c>
-      <c r="C3" s="15">
-        <v>21.212316176470591</v>
-      </c>
-      <c r="D3" s="15">
-        <v>261.88482393355378</v>
-      </c>
-      <c r="E3" s="15">
-        <v>1</v>
-      </c>
-      <c r="F3" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G3" s="15">
-        <v>17.59698113207547</v>
-      </c>
-      <c r="H3" s="15">
-        <v>237.43035975462209</v>
-      </c>
-      <c r="I3" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="14">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>3975</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="15">
+        <v>3264</v>
+      </c>
+      <c r="C4" s="10">
+        <v>9158917.4188146573</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.86643500000000007</v>
+      </c>
+      <c r="E4" s="15">
+        <v>3975</v>
+      </c>
+      <c r="F4" s="10">
+        <v>7520681.0241625998</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.86643500000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="16">
+        <v>3264</v>
+      </c>
+      <c r="C5" s="11">
+        <v>17378481.28444308</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16">
+        <v>3975</v>
+      </c>
+      <c r="F5" s="11">
+        <v>14270028.405640811</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="15">
+        <v>3264</v>
+      </c>
+      <c r="C6" s="10">
+        <v>324271708.62483138</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1.337</v>
+      </c>
+      <c r="E6" s="15">
+        <v>3975</v>
+      </c>
+      <c r="F6" s="10">
+        <v>266269901.35900801</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1.337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="16">
+        <v>3264</v>
+      </c>
+      <c r="C7" s="11">
+        <v>34928920.87043152</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>3975</v>
+      </c>
+      <c r="F7" s="11">
+        <v>28681257.288324151</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="15">
+        <v>3264</v>
+      </c>
+      <c r="C8" s="10">
+        <v>801.29755753707116</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>3975</v>
+      </c>
+      <c r="F8" s="10">
+        <v>657.97112649081771</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="16">
+        <v>3264</v>
+      </c>
+      <c r="C9" s="11">
+        <v>33599.78333427359</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>3975</v>
+      </c>
+      <c r="F9" s="11">
+        <v>27589.85982467145</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="14">
-        <v>3264</v>
-      </c>
-      <c r="C4" s="14">
-        <v>330070050.22725868</v>
-      </c>
-      <c r="D4" s="14">
-        <v>17509100558.713589</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1.337</v>
-      </c>
-      <c r="F4" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G4" s="14">
-        <v>271031105.63330311</v>
-      </c>
-      <c r="H4" s="14">
-        <v>15866175331.40514</v>
-      </c>
-      <c r="I4" s="14">
-        <v>1.337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="15">
-        <v>3264</v>
-      </c>
-      <c r="C5" s="15">
-        <v>35107856.18864923</v>
-      </c>
-      <c r="D5" s="15">
-        <v>1960481387.621767</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0</v>
-      </c>
-      <c r="F5" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G5" s="15">
-        <v>28828186.817547441</v>
-      </c>
-      <c r="H5" s="15">
-        <v>1776518720.275238</v>
-      </c>
-      <c r="I5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="14">
-        <v>3264</v>
-      </c>
-      <c r="C6" s="14">
-        <v>1.2928125619494799</v>
-      </c>
-      <c r="D6" s="14">
-        <v>68.652184320815039</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1.06156986218946</v>
-      </c>
-      <c r="H6" s="14">
-        <v>62.210364045706562</v>
-      </c>
-      <c r="I6" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="15">
-        <v>3264</v>
-      </c>
-      <c r="C7" s="15">
-        <v>2.430759803921569</v>
-      </c>
-      <c r="D7" s="15">
-        <v>41.249932815872953</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0</v>
-      </c>
-      <c r="F7" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G7" s="15">
-        <v>1.9959748427672961</v>
-      </c>
-      <c r="H7" s="15">
-        <v>37.389763944295467</v>
-      </c>
-      <c r="I7" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="14">
-        <v>3264</v>
-      </c>
-      <c r="C8" s="14">
-        <v>5.8927696078431371</v>
-      </c>
-      <c r="D8" s="14">
-        <v>44.419987568039907</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G8" s="14">
-        <v>5.0176100628930822</v>
-      </c>
-      <c r="H8" s="14">
-        <v>40.294327206900583</v>
-      </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="15">
-        <v>3264</v>
-      </c>
-      <c r="C9" s="15">
-        <v>4.520833333333333</v>
-      </c>
-      <c r="D9" s="15">
-        <v>16.485495285444578</v>
-      </c>
-      <c r="E9" s="15">
-        <v>1</v>
-      </c>
-      <c r="F9" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G9" s="15">
-        <v>3.8910691823899368</v>
-      </c>
-      <c r="H9" s="15">
-        <v>14.998975245619789</v>
-      </c>
-      <c r="I9" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>26</v>
       </c>
       <c r="B10" s="15">
         <v>3264</v>
       </c>
-      <c r="C10" s="15">
-        <v>801.29755753707116</v>
-      </c>
-      <c r="D10" s="15">
-        <v>21566.104021791991</v>
+      <c r="C10" s="10">
+        <v>330070050.22725868</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1.337</v>
       </c>
       <c r="E10" s="15">
-        <v>0</v>
-      </c>
-      <c r="F10" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G10" s="15">
-        <v>657.97112649081771</v>
-      </c>
-      <c r="H10" s="15">
-        <v>19544.291501904721</v>
-      </c>
-      <c r="I10" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="14">
+        <v>3975</v>
+      </c>
+      <c r="F10" s="10">
+        <v>271031105.63330311</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1.337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="16">
         <v>3264</v>
       </c>
-      <c r="C11" s="14">
-        <v>324271708.62483138</v>
-      </c>
-      <c r="D11" s="14">
-        <v>17508302812.896229</v>
-      </c>
-      <c r="E11" s="14">
-        <v>1.337</v>
-      </c>
-      <c r="F11" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G11" s="14">
-        <v>266269901.35900801</v>
-      </c>
-      <c r="H11" s="14">
-        <v>15865434919.82373</v>
-      </c>
-      <c r="I11" s="14">
-        <v>1.337</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>28</v>
+      <c r="C11" s="11">
+        <v>35107856.18864923</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16">
+        <v>3975</v>
+      </c>
+      <c r="F11" s="11">
+        <v>28828186.817547441</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B12" s="15">
         <v>3264</v>
       </c>
-      <c r="C12" s="15">
-        <v>9158917.4188146573</v>
-      </c>
-      <c r="D12" s="15">
-        <v>353764014.44052249</v>
+      <c r="C12" s="10">
+        <v>1.2928125619494799</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
       </c>
       <c r="E12" s="15">
-        <v>0.86643500000000007</v>
-      </c>
-      <c r="F12" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G12" s="15">
-        <v>7520681.0241625998</v>
-      </c>
-      <c r="H12" s="15">
-        <v>320578431.63703811</v>
-      </c>
-      <c r="I12" s="15">
-        <v>0.86643500000000007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="14">
+        <v>3975</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1.06156986218946</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="16">
         <v>3264</v>
       </c>
-      <c r="C13" s="14">
-        <v>33599.78333427359</v>
-      </c>
-      <c r="D13" s="14">
-        <v>1754378.05963397</v>
-      </c>
-      <c r="E13" s="14">
-        <v>0</v>
-      </c>
-      <c r="F13" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G13" s="14">
-        <v>27589.85982467145</v>
-      </c>
-      <c r="H13" s="14">
-        <v>1589761.7496576849</v>
-      </c>
-      <c r="I13" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>30</v>
+      <c r="C13" s="11">
+        <v>5.8927696078431371</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16">
+        <v>3975</v>
+      </c>
+      <c r="F13" s="11">
+        <v>5.0176100628930822</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B14" s="15">
         <v>3264</v>
       </c>
-      <c r="C14" s="15">
-        <v>34928920.87043152</v>
-      </c>
-      <c r="D14" s="15">
-        <v>1960473669.1452661</v>
+      <c r="C14" s="10">
+        <v>4.520833333333333</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
       </c>
       <c r="E14" s="15">
-        <v>0</v>
-      </c>
-      <c r="F14" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G14" s="15">
-        <v>28681257.288324151</v>
-      </c>
-      <c r="H14" s="15">
-        <v>1776511208.2888081</v>
-      </c>
-      <c r="I14" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="14">
+        <v>3975</v>
+      </c>
+      <c r="F14" s="10">
+        <v>3.8910691823899368</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="16">
         <v>3264</v>
       </c>
-      <c r="C15" s="14">
-        <v>17378481.28444308</v>
-      </c>
-      <c r="D15" s="14">
-        <v>982815117.76275134</v>
-      </c>
-      <c r="E15" s="14">
-        <v>0</v>
-      </c>
-      <c r="F15" s="14">
-        <v>3975</v>
-      </c>
-      <c r="G15" s="14">
-        <v>14270028.405640811</v>
-      </c>
-      <c r="H15" s="14">
-        <v>890591572.66978121</v>
-      </c>
-      <c r="I15" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>32</v>
+      <c r="C15" s="11">
+        <v>4.465686274509804</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <v>3975</v>
+      </c>
+      <c r="F15" s="11">
+        <v>3.8457861635220132</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B16" s="15">
         <v>3264</v>
       </c>
-      <c r="C16" s="15">
-        <v>1.246936274509804</v>
-      </c>
-      <c r="D16" s="15">
-        <v>6.3174516969443921</v>
+      <c r="C16" s="10">
+        <v>2.430759803921569</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
       </c>
       <c r="E16" s="15">
-        <v>0</v>
-      </c>
-      <c r="F16" s="15">
-        <v>3975</v>
-      </c>
-      <c r="G16" s="15">
-        <v>1.0238993710691819</v>
-      </c>
-      <c r="H16" s="15">
-        <v>5.7444034066363452</v>
-      </c>
-      <c r="I16" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>33</v>
+        <v>3975</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1.9959748427672961</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="B17" s="16">
         <v>3264</v>
       </c>
-      <c r="C17" s="16">
-        <v>4.465686274509804</v>
-      </c>
-      <c r="D17" s="16">
-        <v>16.073423288550451</v>
+      <c r="C17" s="11">
+        <v>1.246936274509804</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
       </c>
       <c r="E17" s="16">
-        <v>1</v>
-      </c>
-      <c r="F17" s="16">
-        <v>3975</v>
-      </c>
-      <c r="G17" s="16">
-        <v>3.8457861635220132</v>
-      </c>
-      <c r="H17" s="16">
-        <v>14.625198925588821</v>
-      </c>
-      <c r="I17" s="16">
+        <v>3975</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1.0238993710691819</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="17">
+        <v>3264</v>
+      </c>
+      <c r="C18" s="12">
+        <v>21.212316176470591</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="17">
+        <v>3975</v>
+      </c>
+      <c r="F18" s="12">
+        <v>17.59698113207547</v>
+      </c>
+      <c r="G18" s="12">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08AFD7D-302B-4FE9-9CA8-8B99A802B665}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="16">
+        <v>584</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="16">
+        <v>702</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <f t="shared" ref="H3:H18" si="0">B3=E3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <f t="shared" ref="I3:I18" si="1">C3=F3</f>
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f>VLOOKUP(A3,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_avg_time_between_contract_tnx</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="15">
+        <v>584</v>
+      </c>
+      <c r="C4" s="10">
+        <v>275307.74940727232</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.70443049999999996</v>
+      </c>
+      <c r="E4" s="15">
+        <v>702</v>
+      </c>
+      <c r="F4" s="10">
+        <v>229031.09386492451</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.86643500000000007</v>
+      </c>
+      <c r="H4" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <f>VLOOKUP(A4,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_avg_val_rec</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="16">
+        <v>584</v>
+      </c>
+      <c r="C5" s="11">
+        <v>24484.908842929799</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16">
+        <v>702</v>
+      </c>
+      <c r="F5" s="11">
+        <v>20369.211914915959</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
+        <f>VLOOKUP(A5,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_avg_val_sent</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="15">
+        <v>584</v>
+      </c>
+      <c r="C6" s="10">
+        <v>8970138.6947486028</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1.1845954999999999</v>
+      </c>
+      <c r="E6" s="15">
+        <v>702</v>
+      </c>
+      <c r="F6" s="10">
+        <v>7462337.8283464154</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1.337</v>
+      </c>
+      <c r="H6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
+        <f>VLOOKUP(A6,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_max_val_rec</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="16">
+        <v>584</v>
+      </c>
+      <c r="C7" s="11">
+        <v>516769.25731442968</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>702</v>
+      </c>
+      <c r="F7" s="11">
+        <v>429904.90921884181</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" t="str">
+        <f>VLOOKUP(A7,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_max_val_sent</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="15">
+        <v>584</v>
+      </c>
+      <c r="C8" s="10">
+        <v>286.51782083047942</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>702</v>
+      </c>
+      <c r="F8" s="10">
+        <v>238.35670564814811</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
+        <f>VLOOKUP(A8,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_min_val_rec</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="16">
+        <v>584</v>
+      </c>
+      <c r="C9" s="11">
+        <v>331.59041736130138</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>702</v>
+      </c>
+      <c r="F9" s="11">
+        <v>275.85299677920227</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <f>VLOOKUP(A9,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_min_val_sent</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="15">
+        <v>584</v>
+      </c>
+      <c r="C10" s="10">
+        <v>16279877.061012451</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1.337</v>
+      </c>
+      <c r="E10" s="15">
+        <v>702</v>
+      </c>
+      <c r="F10" s="10">
+        <v>13543373.73418414</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1.337</v>
+      </c>
+      <c r="H10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" t="str">
+        <f>VLOOKUP(A10,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_total_Ether_received</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="16">
+        <v>584</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1302267.1333386039</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16">
+        <v>702</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1083367.529728981</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" t="str">
+        <f>VLOOKUP(A11,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_total_ether_sent</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="15">
+        <v>584</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1669.6844347602739</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="15">
+        <v>702</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1389.0252277777779</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" t="str">
+        <f>VLOOKUP(A12,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_total_Ether_sent_contract</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="16">
+        <v>584</v>
+      </c>
+      <c r="C13" s="11">
+        <v>5.4315068493150687</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16">
+        <v>702</v>
+      </c>
+      <c r="F13" s="11">
+        <v>4.6866096866096862</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" t="str">
+        <f>VLOOKUP(A13,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_uniq_rec_addr</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="15">
+        <v>584</v>
+      </c>
+      <c r="C14" s="10">
+        <v>4.4486301369863011</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="15">
+        <v>702</v>
+      </c>
+      <c r="F14" s="10">
+        <v>3.8689458689458691</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" t="str">
+        <f>VLOOKUP(A14,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_uniq_rec_contract_addr</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="16">
+        <v>584</v>
+      </c>
+      <c r="C15" s="11">
+        <v>4.3561643835616426</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <v>702</v>
+      </c>
+      <c r="F15" s="11">
+        <v>3.792022792022792</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" t="str">
+        <f>VLOOKUP(A15,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_uniq_rec_token_name</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="15">
+        <v>584</v>
+      </c>
+      <c r="C16" s="10">
+        <v>3.7260273972602742</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15">
+        <v>702</v>
+      </c>
+      <c r="F16" s="10">
+        <v>3.0997150997151</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" t="str">
+        <f>VLOOKUP(A16,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_uniq_sent_addr</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="16">
+        <v>584</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1.203767123287671</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="16">
+        <v>702</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1.0014245014245009</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" t="str">
+        <f>VLOOKUP(A17,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>ERC20_uniq_sent_token_name</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="17">
+        <v>584</v>
+      </c>
+      <c r="C18" s="12">
+        <v>29.604452054794521</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="17">
+        <v>702</v>
+      </c>
+      <c r="F18" s="12">
+        <v>24.796296296296301</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18" t="e">
+        <f>VLOOKUP(A18,'SOMENTE ALTERADAS'!$A$3:$A$17,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE76DE5-2D1C-474D-8876-27955126AC61}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65781947-C16C-4F97-B001-70C06EE8A5C1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>